<commit_message>
fixed some labels in example forms
</commit_message>
<xml_diff>
--- a/public/forms/building_placeholders.xlsx
+++ b/public/forms/building_placeholders.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="196">
   <si>
     <t>type</t>
   </si>
@@ -723,17 +723,17 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="1" sqref="C103:C108 F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,14 +854,14 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="C103:C108 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.2244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.015306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.7551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.24489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,16 +894,16 @@
   </sheetPr>
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C103" activeCellId="0" sqref="C103:C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2244897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9132653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.24489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1925,6 +1925,9 @@
       <c r="B103" s="0" t="s">
         <v>189</v>
       </c>
+      <c r="C103" s="0" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
@@ -1933,6 +1936,9 @@
       <c r="B104" s="0" t="s">
         <v>190</v>
       </c>
+      <c r="C104" s="0" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
@@ -1941,6 +1947,9 @@
       <c r="B105" s="0" t="s">
         <v>191</v>
       </c>
+      <c r="C105" s="0" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
@@ -1952,12 +1961,18 @@
       <c r="B107" s="0" t="s">
         <v>192</v>
       </c>
+      <c r="C107" s="0" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B108" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C108" s="0" t="s">
         <v>193</v>
       </c>
     </row>
@@ -1980,14 +1995,14 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C103:C108 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.48469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>